<commit_message>
added multiprocessing code (tested)
</commit_message>
<xml_diff>
--- a/collect data/running.xlsx
+++ b/collect data/running.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\courses\thesis preparation\new model reference model\collect data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10EED1F-4371-4910-9814-0DEBBA54B51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50082D57-5395-4955-A8A1-628F0D076850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:AM812"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q315" workbookViewId="0">
-      <selection activeCell="AI325" sqref="AI325"/>
+      <selection activeCell="AF328" sqref="AF328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>